<commit_message>
Calc functions working on different models
</commit_message>
<xml_diff>
--- a/Decision Matrices/dummy_drone_data.xlsx
+++ b/Decision Matrices/dummy_drone_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc3adef44a32c2c0/Documents/GitHub/DP4/Decision Matrices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{26A6A077-90E6-46C6-B193-06E9AC2A7034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D8B9F57-2AD9-41D0-A524-80DCFC28030F}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="8_{26A6A077-90E6-46C6-B193-06E9AC2A7034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEBCADE4-A355-4F4D-B41D-0624F7611669}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{392446B4-2555-431B-ACD7-CFCCCB762E0C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Company</t>
   </si>
@@ -71,30 +71,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>numeric</t>
-  </si>
-  <si>
-    <t>discrete</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>maximise</t>
-  </si>
-  <si>
-    <t>minimise</t>
-  </si>
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t>OBJECTIVE</t>
-  </si>
-  <si>
-    <t>match job</t>
-  </si>
-  <si>
     <t>Payload</t>
   </si>
   <si>
@@ -132,6 +108,30 @@
   </si>
   <si>
     <t>Cargo space</t>
+  </si>
+  <si>
+    <t>Company 1</t>
+  </si>
+  <si>
+    <t>Model 1</t>
+  </si>
+  <si>
+    <t>Company 2</t>
+  </si>
+  <si>
+    <t>Model 2</t>
+  </si>
+  <si>
+    <t>Company 3</t>
+  </si>
+  <si>
+    <t>Model 3</t>
+  </si>
+  <si>
+    <t>Company 4</t>
+  </si>
+  <si>
+    <t>Model 4</t>
   </si>
 </sst>
 </file>
@@ -147,9 +147,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -175,9 +173,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,18 +489,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5198C466-9594-45C2-881A-0055B522FAA5}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="B1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G4" sqref="F4:W4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -520,40 +520,40 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="R1" t="s">
         <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R1" t="s">
-        <v>28</v>
       </c>
       <c r="S1" t="s">
         <v>6</v>
@@ -565,136 +565,157 @@
         <v>8</v>
       </c>
       <c r="V1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>11</v>
-      </c>
-      <c r="R2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S2" t="s">
-        <v>12</v>
-      </c>
-      <c r="T2" t="s">
-        <v>12</v>
-      </c>
-      <c r="U2" t="s">
-        <v>13</v>
-      </c>
-      <c r="V2" t="s">
-        <v>11</v>
-      </c>
-      <c r="W2" t="s">
-        <v>11</v>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+      <c r="R2">
+        <v>2</v>
+      </c>
+      <c r="S2">
+        <v>2</v>
+      </c>
+      <c r="T2">
+        <v>9</v>
+      </c>
+      <c r="U2">
+        <v>9</v>
+      </c>
+      <c r="V2">
+        <v>2</v>
+      </c>
+      <c r="W2">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S3" t="s">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="T3" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="U3" t="s">
-        <v>10</v>
-      </c>
-      <c r="V3" t="s">
-        <v>15</v>
-      </c>
-      <c r="W3" t="s">
-        <v>15</v>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <v>3</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3">
+        <v>9</v>
+      </c>
+      <c r="U3">
+        <v>9</v>
+      </c>
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3">
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -703,83 +724,127 @@
         <v>10</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="U4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="V4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <v>5</v>
+      </c>
+      <c r="O5">
+        <v>5</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
+      </c>
+      <c r="Q5">
+        <v>5</v>
+      </c>
+      <c r="R5">
+        <v>5</v>
+      </c>
+      <c r="S5">
+        <v>5</v>
+      </c>
+      <c r="T5">
+        <v>9</v>
+      </c>
+      <c r="U5">
+        <v>9</v>
+      </c>
+      <c r="V5">
+        <v>5</v>
+      </c>
+      <c r="W5">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>